<commit_message>
Moving active version of spreadsheet to Google Drive
</commit_message>
<xml_diff>
--- a/v1/galls_2022/DATA/Global Cynipini host oak list 20220520.xlsx
+++ b/v1/galls_2022/DATA/Global Cynipini host oak list 20220520.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Dropbox\FAGACEAE-elliot\DATA.AND.TREES\2022 - Graham tree\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\fagaceae-phylo\v1\galls_2022\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B020FEB-6ABD-47E6-95AB-38459CD85C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A106A058-6E86-49EA-BD4B-644D8D6F879B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{80D947C2-EB75-4A17-AF8D-C5681FF4B280}"/>
   </bookViews>
@@ -29,8 +29,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -57,106 +57,223 @@
   <commentList>
     <comment ref="A32" authorId="0" shapeId="0" xr:uid="{E379B108-040E-493B-B947-463FB2AF1611}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     wikipedia thinks this isn't a species; Denk et al seem to</t>
+        </r>
       </text>
     </comment>
     <comment ref="A40" authorId="1" shapeId="0" xr:uid="{E19E7F26-7328-453C-B223-C62B5ED52788}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     incl Q persica</t>
+        </r>
       </text>
     </comment>
     <comment ref="A45" authorId="2" shapeId="0" xr:uid="{134E65E9-0B67-43AD-9E91-1EFCD91995CA}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     incl Q. gussonei</t>
+        </r>
       </text>
     </comment>
     <comment ref="A67" authorId="3" shapeId="0" xr:uid="{939E1FF7-F9AA-4BAD-8583-1014C4724602}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Q. x undulata is gambelii + grisea (oaknames.org). Q. x fendleri is itself a syn of maybe that or else Q. x pauciloba (gambelii + turbinella). Q. utahensis is a syn.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A78" authorId="4" shapeId="0" xr:uid="{552672B8-EA2C-4C3D-A3BD-FA087A4757C8}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Q. x undulata is gambelii x grisea (oaknames.org)</t>
+        </r>
       </text>
     </comment>
     <comment ref="A109" authorId="5" shapeId="0" xr:uid="{7868DF2D-FCB6-46B6-8B7C-D9DD80A11704}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     potentially includes records from Q. prinus</t>
+        </r>
       </text>
     </comment>
     <comment ref="A113" authorId="6" shapeId="0" xr:uid="{BD477ADD-FDCB-42FE-847A-EB801A798E1B}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     incl some Q. prinus records</t>
+        </r>
       </text>
     </comment>
     <comment ref="A127" authorId="7" shapeId="0" xr:uid="{0CA23B43-C516-415A-8330-716BB2332EBE}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Denk et al list this as section Quercus but they must be wrong! oaknames.org says it's Lobatae (as does wikipedia)</t>
+        </r>
       </text>
     </comment>
     <comment ref="A141" authorId="8" shapeId="0" xr:uid="{E6284D5E-206C-4DE7-B692-420A31028199}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     =Q. reticulata (syn); =Q. rhodophlebia (syn)</t>
+        </r>
       </text>
     </comment>
     <comment ref="A145" authorId="9" shapeId="0" xr:uid="{95F52CF0-29ED-44BA-A998-8DA8B0E2E635}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     includes Q. bumelioides</t>
+        </r>
       </text>
     </comment>
     <comment ref="A149" authorId="10" shapeId="0" xr:uid="{F876E841-F90D-4B07-9829-9E68E8066A39}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     includes Q. durandii and Q. breviloba</t>
+        </r>
       </text>
     </comment>
     <comment ref="M151" authorId="11" shapeId="0" xr:uid="{68FEF723-9273-4866-BB7E-D4F0D21158C0}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     some disagreement - splendens isn't accepted by Denk or oaknames.org but is by worldfloraonline.org</t>
+        </r>
       </text>
     </comment>
     <comment ref="A167" authorId="12" shapeId="0" xr:uid="{5271C095-D8CA-4B02-B369-68D7DE7664C8}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     =wutaishansea [sic]</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1982,25 +2099,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5ED4142-E336-484E-BDA7-D821A2E296CD}">
   <dimension ref="A1:M168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="16.08984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="41.36328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.31640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.6796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="104.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="16.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="41.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="104.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2041,7 +2158,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>154</v>
       </c>
@@ -2075,7 +2192,7 @@
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>155</v>
       </c>
@@ -2100,7 +2217,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>156</v>
       </c>
@@ -2125,7 +2242,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>157</v>
       </c>
@@ -2150,7 +2267,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>158</v>
       </c>
@@ -2175,7 +2292,7 @@
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>179</v>
       </c>
@@ -2207,7 +2324,7 @@
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>175</v>
       </c>
@@ -2232,7 +2349,7 @@
       </c>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>159</v>
       </c>
@@ -2257,7 +2374,7 @@
       </c>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>167</v>
       </c>
@@ -2282,7 +2399,7 @@
       </c>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>170</v>
       </c>
@@ -2308,7 +2425,7 @@
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>160</v>
       </c>
@@ -2333,7 +2450,7 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
@@ -2358,7 +2475,7 @@
       </c>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>165</v>
       </c>
@@ -2390,7 +2507,7 @@
       </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
@@ -2422,7 +2539,7 @@
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="14.75" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="16" spans="1:13" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>161</v>
       </c>
@@ -2448,7 +2565,7 @@
       </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -2473,7 +2590,7 @@
       </c>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>168</v>
       </c>
@@ -2499,7 +2616,7 @@
       </c>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>171</v>
       </c>
@@ -2525,7 +2642,7 @@
       </c>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" ht="14.75" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="20" spans="1:13" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>129</v>
       </c>
@@ -2551,7 +2668,7 @@
       </c>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>173</v>
       </c>
@@ -2576,7 +2693,7 @@
       </c>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>174</v>
       </c>
@@ -2601,7 +2718,7 @@
       </c>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>176</v>
       </c>
@@ -2627,7 +2744,7 @@
       </c>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" ht="14.75" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="24" spans="1:13" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>130</v>
       </c>
@@ -2653,7 +2770,7 @@
       </c>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>172</v>
       </c>
@@ -2678,7 +2795,7 @@
       </c>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>169</v>
       </c>
@@ -2704,7 +2821,7 @@
       </c>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>399</v>
       </c>
@@ -2730,7 +2847,7 @@
       </c>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>31</v>
       </c>
@@ -2755,7 +2872,7 @@
       </c>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>32</v>
       </c>
@@ -2780,7 +2897,7 @@
       </c>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>138</v>
       </c>
@@ -2805,7 +2922,7 @@
       </c>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>33</v>
       </c>
@@ -2830,7 +2947,7 @@
       </c>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
@@ -2855,7 +2972,7 @@
       </c>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
@@ -2880,7 +2997,7 @@
       </c>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>131</v>
       </c>
@@ -2905,7 +3022,7 @@
       </c>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>177</v>
       </c>
@@ -2939,7 +3056,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="118" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>140</v>
       </c>
@@ -2975,7 +3092,7 @@
       </c>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>36</v>
       </c>
@@ -3000,7 +3117,7 @@
       </c>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>37</v>
       </c>
@@ -3025,7 +3142,7 @@
       </c>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>38</v>
       </c>
@@ -3050,7 +3167,7 @@
       </c>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>15</v>
       </c>
@@ -3075,7 +3192,7 @@
       </c>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>39</v>
       </c>
@@ -3100,7 +3217,7 @@
       </c>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>2</v>
       </c>
@@ -3125,7 +3242,7 @@
       </c>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>40</v>
       </c>
@@ -3150,7 +3267,7 @@
       </c>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>16</v>
       </c>
@@ -3175,7 +3292,7 @@
       </c>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>17</v>
       </c>
@@ -3200,7 +3317,7 @@
       </c>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>41</v>
       </c>
@@ -3225,7 +3342,7 @@
       </c>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>42</v>
       </c>
@@ -3250,7 +3367,7 @@
       </c>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>43</v>
       </c>
@@ -3275,7 +3392,7 @@
       </c>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>18</v>
       </c>
@@ -3300,7 +3417,7 @@
       </c>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>44</v>
       </c>
@@ -3325,7 +3442,7 @@
       </c>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>45</v>
       </c>
@@ -3350,7 +3467,7 @@
       </c>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>46</v>
       </c>
@@ -3375,7 +3492,7 @@
       </c>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>3</v>
       </c>
@@ -3400,7 +3517,7 @@
       </c>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>132</v>
       </c>
@@ -3425,7 +3542,7 @@
       </c>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>47</v>
       </c>
@@ -3450,7 +3567,7 @@
       </c>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>48</v>
       </c>
@@ -3475,7 +3592,7 @@
       </c>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>49</v>
       </c>
@@ -3500,7 +3617,7 @@
       </c>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>50</v>
       </c>
@@ -3525,7 +3642,7 @@
       </c>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>51</v>
       </c>
@@ -3550,7 +3667,7 @@
       </c>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>52</v>
       </c>
@@ -3575,7 +3692,7 @@
       </c>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>53</v>
       </c>
@@ -3600,7 +3717,7 @@
       </c>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>133</v>
       </c>
@@ -3625,7 +3742,7 @@
       </c>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>4</v>
       </c>
@@ -3650,7 +3767,7 @@
       </c>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>54</v>
       </c>
@@ -3675,7 +3792,7 @@
       </c>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>5</v>
       </c>
@@ -3700,7 +3817,7 @@
       </c>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>55</v>
       </c>
@@ -3725,7 +3842,7 @@
       </c>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="1:13" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>56</v>
       </c>
@@ -3761,7 +3878,7 @@
       </c>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>182</v>
       </c>
@@ -3788,7 +3905,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>57</v>
       </c>
@@ -3813,7 +3930,7 @@
       </c>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
         <v>58</v>
       </c>
@@ -3838,7 +3955,7 @@
       </c>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>59</v>
       </c>
@@ -3863,7 +3980,7 @@
       </c>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
         <v>144</v>
       </c>
@@ -3888,7 +4005,7 @@
       </c>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>60</v>
       </c>
@@ -3913,7 +4030,7 @@
       </c>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
         <v>145</v>
       </c>
@@ -3938,7 +4055,7 @@
       </c>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>61</v>
       </c>
@@ -3963,7 +4080,7 @@
       </c>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>181</v>
       </c>
@@ -3992,7 +4109,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>134</v>
       </c>
@@ -4017,7 +4134,7 @@
       </c>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>62</v>
       </c>
@@ -4042,7 +4159,7 @@
       </c>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>6</v>
       </c>
@@ -4067,7 +4184,7 @@
       </c>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>63</v>
       </c>
@@ -4094,7 +4211,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>64</v>
       </c>
@@ -4119,7 +4236,7 @@
       </c>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>65</v>
       </c>
@@ -4144,7 +4261,7 @@
       </c>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>66</v>
       </c>
@@ -4169,7 +4286,7 @@
       </c>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="1:13" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>146</v>
       </c>
@@ -4196,7 +4313,7 @@
       </c>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>19</v>
       </c>
@@ -4221,7 +4338,7 @@
       </c>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>67</v>
       </c>
@@ -4246,7 +4363,7 @@
       </c>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>68</v>
       </c>
@@ -4271,7 +4388,7 @@
       </c>
       <c r="M87" s="1"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>69</v>
       </c>
@@ -4296,7 +4413,7 @@
       </c>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>7</v>
       </c>
@@ -4321,7 +4438,7 @@
       </c>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>70</v>
       </c>
@@ -4346,7 +4463,7 @@
       </c>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
         <v>20</v>
       </c>
@@ -4371,7 +4488,7 @@
       </c>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>71</v>
       </c>
@@ -4396,7 +4513,7 @@
       </c>
       <c r="M92" s="1"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>72</v>
       </c>
@@ -4421,7 +4538,7 @@
       </c>
       <c r="M93" s="1"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>73</v>
       </c>
@@ -4446,7 +4563,7 @@
       </c>
       <c r="M94" s="1"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>74</v>
       </c>
@@ -4471,7 +4588,7 @@
       </c>
       <c r="M95" s="1"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>75</v>
       </c>
@@ -4496,7 +4613,7 @@
       </c>
       <c r="M96" s="1"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>76</v>
       </c>
@@ -4521,7 +4638,7 @@
       </c>
       <c r="M97" s="1"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>77</v>
       </c>
@@ -4546,7 +4663,7 @@
       </c>
       <c r="M98" s="1"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="16" t="s">
         <v>21</v>
       </c>
@@ -4571,7 +4688,7 @@
       </c>
       <c r="M99" s="1"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>78</v>
       </c>
@@ -4596,7 +4713,7 @@
       </c>
       <c r="M100" s="1"/>
     </row>
-    <row r="101" spans="1:13" ht="59" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
         <v>147</v>
       </c>
@@ -4632,7 +4749,7 @@
       </c>
       <c r="M101" s="1"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>8</v>
       </c>
@@ -4657,7 +4774,7 @@
       </c>
       <c r="M102" s="1"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>79</v>
       </c>
@@ -4682,7 +4799,7 @@
       </c>
       <c r="M103" s="1"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>9</v>
       </c>
@@ -4707,7 +4824,7 @@
       </c>
       <c r="M104" s="1"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>80</v>
       </c>
@@ -4732,7 +4849,7 @@
       </c>
       <c r="M105" s="1"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>81</v>
       </c>
@@ -4757,7 +4874,7 @@
       </c>
       <c r="M106" s="1"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>82</v>
       </c>
@@ -4782,7 +4899,7 @@
       </c>
       <c r="M107" s="1"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>83</v>
       </c>
@@ -4807,7 +4924,7 @@
       </c>
       <c r="M108" s="1"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>84</v>
       </c>
@@ -4832,7 +4949,7 @@
       </c>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="19" t="s">
         <v>85</v>
       </c>
@@ -4857,7 +4974,7 @@
       </c>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>135</v>
       </c>
@@ -4882,7 +4999,7 @@
       </c>
       <c r="M111" s="1"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>141</v>
       </c>
@@ -4907,7 +5024,7 @@
       </c>
       <c r="M112" s="1"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>86</v>
       </c>
@@ -4932,7 +5049,7 @@
       </c>
       <c r="M113" s="1"/>
     </row>
-    <row r="114" spans="1:13" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
         <v>148</v>
       </c>
@@ -4968,7 +5085,7 @@
       </c>
       <c r="M114" s="1"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="s">
         <v>183</v>
       </c>
@@ -4995,7 +5112,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="s">
         <v>184</v>
       </c>
@@ -5020,7 +5137,7 @@
       </c>
       <c r="M116" s="1"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>88</v>
       </c>
@@ -5045,7 +5162,7 @@
       </c>
       <c r="M117" s="1"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
         <v>89</v>
       </c>
@@ -5070,7 +5187,7 @@
       </c>
       <c r="M118" s="1"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>90</v>
       </c>
@@ -5095,7 +5212,7 @@
       </c>
       <c r="M119" s="1"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>91</v>
       </c>
@@ -5120,7 +5237,7 @@
       </c>
       <c r="M120" s="1"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="19" t="s">
         <v>92</v>
       </c>
@@ -5145,7 +5262,7 @@
       </c>
       <c r="M121" s="1"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="s">
         <v>178</v>
       </c>
@@ -5170,7 +5287,7 @@
       </c>
       <c r="M122" s="1"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>93</v>
       </c>
@@ -5195,7 +5312,7 @@
       </c>
       <c r="M123" s="1"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>94</v>
       </c>
@@ -5220,7 +5337,7 @@
       </c>
       <c r="M124" s="1"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>95</v>
       </c>
@@ -5245,7 +5362,7 @@
       </c>
       <c r="M125" s="1"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>96</v>
       </c>
@@ -5270,7 +5387,7 @@
       </c>
       <c r="M126" s="1"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>97</v>
       </c>
@@ -5295,7 +5412,7 @@
       </c>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>10</v>
       </c>
@@ -5320,7 +5437,7 @@
       </c>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>98</v>
       </c>
@@ -5345,7 +5462,7 @@
       </c>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>99</v>
       </c>
@@ -5370,7 +5487,7 @@
       </c>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="22" t="s">
         <v>11</v>
       </c>
@@ -5395,7 +5512,7 @@
       </c>
       <c r="M131" s="1"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>100</v>
       </c>
@@ -5420,7 +5537,7 @@
       </c>
       <c r="M132" s="1"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>101</v>
       </c>
@@ -5445,7 +5562,7 @@
       </c>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>12</v>
       </c>
@@ -5470,7 +5587,7 @@
       </c>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>102</v>
       </c>
@@ -5495,7 +5612,7 @@
       </c>
       <c r="M135" s="1"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>103</v>
       </c>
@@ -5520,7 +5637,7 @@
       </c>
       <c r="M136" s="1"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>13</v>
       </c>
@@ -5545,7 +5662,7 @@
       </c>
       <c r="M137" s="1"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>104</v>
       </c>
@@ -5570,7 +5687,7 @@
       </c>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>14</v>
       </c>
@@ -5595,7 +5712,7 @@
       </c>
       <c r="M139" s="1"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>105</v>
       </c>
@@ -5620,7 +5737,7 @@
       </c>
       <c r="M140" s="1"/>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>106</v>
       </c>
@@ -5645,7 +5762,7 @@
       </c>
       <c r="M141" s="1"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="22" t="s">
         <v>107</v>
       </c>
@@ -5670,7 +5787,7 @@
       </c>
       <c r="M142" s="1"/>
     </row>
-    <row r="143" spans="1:13" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>108</v>
       </c>
@@ -5706,7 +5823,7 @@
       </c>
       <c r="M143" s="1"/>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="21" t="s">
         <v>149</v>
       </c>
@@ -5731,7 +5848,7 @@
       </c>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>109</v>
       </c>
@@ -5756,7 +5873,7 @@
       </c>
       <c r="M145" s="1"/>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>136</v>
       </c>
@@ -5781,7 +5898,7 @@
       </c>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="21" t="s">
         <v>150</v>
       </c>
@@ -5806,7 +5923,7 @@
       </c>
       <c r="M147" s="1"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
         <v>110</v>
       </c>
@@ -5831,7 +5948,7 @@
       </c>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>111</v>
       </c>
@@ -5856,7 +5973,7 @@
       </c>
       <c r="M149" s="1"/>
     </row>
-    <row r="150" spans="1:13" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
         <v>142</v>
       </c>
@@ -5894,7 +6011,7 @@
       </c>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>112</v>
       </c>
@@ -5930,7 +6047,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>113</v>
       </c>
@@ -5955,7 +6072,7 @@
       </c>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="23" t="s">
         <v>22</v>
       </c>
@@ -5980,7 +6097,7 @@
       </c>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="1:13" ht="132.75" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A154" s="15" t="s">
         <v>143</v>
       </c>
@@ -6010,7 +6127,7 @@
       </c>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
         <v>125</v>
       </c>
@@ -6035,7 +6152,7 @@
       </c>
       <c r="M155" s="1"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
         <v>114</v>
       </c>
@@ -6060,7 +6177,7 @@
       </c>
       <c r="M156" s="1"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>115</v>
       </c>
@@ -6085,7 +6202,7 @@
       </c>
       <c r="M157" s="1"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
         <v>23</v>
       </c>
@@ -6110,7 +6227,7 @@
       </c>
       <c r="M158" s="1"/>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>116</v>
       </c>
@@ -6135,7 +6252,7 @@
       </c>
       <c r="M159" s="1"/>
     </row>
-    <row r="160" spans="1:13" ht="221.25" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>117</v>
       </c>
@@ -6170,7 +6287,7 @@
       </c>
       <c r="M160" s="1"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="17" t="s">
         <v>118</v>
       </c>
@@ -6197,7 +6314,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="24" t="s">
         <v>166</v>
       </c>
@@ -6222,7 +6339,7 @@
       </c>
       <c r="M162" s="1"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>139</v>
       </c>
@@ -6249,7 +6366,7 @@
       </c>
       <c r="M163" s="1"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>119</v>
       </c>
@@ -6274,7 +6391,7 @@
       </c>
       <c r="M164" s="1"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="19" t="s">
         <v>120</v>
       </c>
@@ -6299,7 +6416,7 @@
       </c>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>121</v>
       </c>
@@ -6324,7 +6441,7 @@
       </c>
       <c r="M166" s="1"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>137</v>
       </c>
@@ -6351,7 +6468,7 @@
       </c>
       <c r="M167" s="1"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>87</v>
       </c>
@@ -6379,7 +6496,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M168">
+  <sortState ref="A2:M168">
     <sortCondition ref="A15:A168"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>